<commit_message>
Updating keras sheet bugs
</commit_message>
<xml_diff>
--- a/Keras Bugs Sheets.xlsx
+++ b/Keras Bugs Sheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tempo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF7A423-0E2F-4F09-AD2D-1671BAEF4C14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61161909-0632-410D-A6D7-842E3F4776AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues Voting" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5100" uniqueCount="3234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5103" uniqueCount="3239">
   <si>
     <t>Title</t>
   </si>
@@ -9507,9 +9507,6 @@
   </si>
   <si>
     <t>tf.keras renaming import</t>
-  </si>
-  <si>
-    <t>gist is not accessible</t>
   </si>
   <si>
     <t>1.15.0-dev20190731</t>
@@ -9806,9 +9803,6 @@
     </r>
   </si>
   <si>
-    <t>Same as error 6</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">TF Nightly. Gist: </t>
     </r>
@@ -9894,9 +9888,6 @@
       </rPr>
       <t>https://colab.research.google.com/gist/jvishnuvardhan/7e5689d9d23203acd54f266b8e88a35d/untitled765.ipynb</t>
     </r>
-  </si>
-  <si>
-    <t>Same as 18</t>
   </si>
   <si>
     <r>
@@ -10254,6 +10245,30 @@
   </si>
   <si>
     <t>Note: Issue in red are removed issue</t>
+  </si>
+  <si>
+    <t>Reason for rejection: The users don't actually agree the issue is closed, even if it is marked as such. A new will be open</t>
+  </si>
+  <si>
+    <t>Reason for rejection: Same as error 6 (Duplicate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reason for rejection: Not a bug it seems, more like user didn't using it correctly. However, as he mentionned, there should be a mechanism to raise mismatch of dimension. </t>
+  </si>
+  <si>
+    <t>Reason for rejection: Same as 18 (Duplicate)</t>
+  </si>
+  <si>
+    <t>Reason for rejection: Not actually a bug after further inspection, seems to be the user trying to use a functionality that doesn't exist</t>
+  </si>
+  <si>
+    <t>Reason for rejection: Same as 50 (Duplicate)</t>
+  </si>
+  <si>
+    <t>None (but user tracked down error and opened a pull request)</t>
+  </si>
+  <si>
+    <t>None (but user tracked down error)</t>
   </si>
 </sst>
 </file>
@@ -10628,10 +10643,10 @@
     <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10852,9 +10867,9 @@
   </sheetPr>
   <dimension ref="A1:Q1175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1167" sqref="F1167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10879,20 +10894,20 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="82" t="s">
-        <v>3230</v>
+      <c r="D1" s="81" t="s">
+        <v>3227</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="82" t="s">
-        <v>3231</v>
+      <c r="F1" s="81" t="s">
+        <v>3228</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="82" t="s">
-        <v>3231</v>
+      <c r="H1" s="81" t="s">
+        <v>3228</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>3</v>
@@ -10901,7 +10916,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5" t="s">
-        <v>3227</v>
+        <v>3224</v>
       </c>
       <c r="N1" s="6"/>
       <c r="O1" s="5"/>
@@ -43556,10 +43571,10 @@
     </row>
     <row r="1171" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I1171" t="s">
-        <v>3228</v>
+        <v>3225</v>
       </c>
       <c r="J1171" t="s">
-        <v>3229</v>
+        <v>3226</v>
       </c>
     </row>
     <row r="1172" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -44774,6 +44789,7 @@
     <hyperlink ref="B1169" r:id="rId1172" xr:uid="{15EDCEC0-B72E-4D57-A4AC-7DDC17F78945}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1173"/>
 </worksheet>
 </file>
 
@@ -44813,16 +44829,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="22" t="s">
+        <v>3182</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>3183</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>3184</v>
+      </c>
+      <c r="H1" s="22" t="s">
         <v>3185</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>3186</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>3187</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>3188</v>
       </c>
       <c r="J1" s="11"/>
     </row>
@@ -44867,13 +44883,13 @@
         <v>234</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>3189</v>
+        <v>3186</v>
       </c>
       <c r="H3" s="11" t="b">
         <v>1</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>3190</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -44894,16 +44910,16 @@
         <v>239</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>3191</v>
+        <v>3188</v>
       </c>
       <c r="H4" s="12" t="b">
         <v>0</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>3192</v>
+        <v>3189</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>3193</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -44923,13 +44939,13 @@
         <v>251</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>3194</v>
+        <v>3191</v>
       </c>
       <c r="H5" s="11" t="b">
         <v>1</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>3195</v>
+        <v>3192</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -44952,13 +44968,13 @@
         <v>256</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>3196</v>
+        <v>3193</v>
       </c>
       <c r="H6" s="11" t="b">
         <v>1</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>3197</v>
+        <v>3194</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -44981,13 +44997,13 @@
         <v>277</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>3198</v>
+        <v>3195</v>
       </c>
       <c r="H7" s="12" t="b">
         <v>0</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>3199</v>
+        <v>3196</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -45049,7 +45065,7 @@
         <v>399</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>3200</v>
+        <v>3197</v>
       </c>
       <c r="H10" s="11" t="b">
         <v>1</v>
@@ -45072,13 +45088,13 @@
         <v>426</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>3201</v>
+        <v>3198</v>
       </c>
       <c r="H11" s="12" t="b">
         <v>0</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>3202</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -45098,7 +45114,7 @@
         <v>454</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>3203</v>
+        <v>3200</v>
       </c>
       <c r="H12" s="11" t="b">
         <v>1</v>
@@ -45119,7 +45135,7 @@
         <v>464</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>3204</v>
+        <v>3201</v>
       </c>
       <c r="H13" s="11" t="b">
         <v>1</v>
@@ -45142,7 +45158,7 @@
         <v>476</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>3205</v>
+        <v>3202</v>
       </c>
       <c r="H14" s="11" t="b">
         <v>1</v>
@@ -45171,7 +45187,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>3206</v>
+        <v>3203</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -45223,10 +45239,10 @@
         <v>0</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>3207</v>
+        <v>3204</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>3208</v>
+        <v>3205</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
@@ -45252,7 +45268,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>3209</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
@@ -45278,10 +45294,10 @@
         <v>0</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>3210</v>
+        <v>3207</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>3211</v>
+        <v>3208</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
@@ -45307,7 +45323,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>3209</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
@@ -45324,7 +45340,7 @@
         <v>2269</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>3212</v>
+        <v>3209</v>
       </c>
       <c r="H21" s="11" t="b">
         <v>1</v>
@@ -45347,7 +45363,7 @@
         <v>2293</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>3212</v>
+        <v>3209</v>
       </c>
       <c r="H22" s="11" t="b">
         <v>1</v>
@@ -45393,7 +45409,7 @@
         <v>2136</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>3212</v>
+        <v>3209</v>
       </c>
       <c r="H24" s="11" t="b">
         <v>1</v>
@@ -45419,7 +45435,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>3209</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
@@ -45439,7 +45455,7 @@
         <v>2412</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>3212</v>
+        <v>3209</v>
       </c>
       <c r="H26" s="11" t="b">
         <v>1</v>
@@ -45469,10 +45485,10 @@
         <v>0</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>3213</v>
+        <v>3210</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>3214</v>
+        <v>3211</v>
       </c>
       <c r="K27" s="19"/>
       <c r="L27" s="19"/>
@@ -45503,7 +45519,7 @@
         <v>2412</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>3212</v>
+        <v>3209</v>
       </c>
       <c r="H28" s="11" t="b">
         <v>1</v>
@@ -45520,7 +45536,7 @@
         <v>1773</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>3215</v>
+        <v>3212</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>2462</v>
@@ -45535,7 +45551,7 @@
         <v>1910</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>3216</v>
+        <v>3213</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
@@ -45555,7 +45571,7 @@
         <v>2412</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>3212</v>
+        <v>3209</v>
       </c>
       <c r="H30" s="11" t="b">
         <v>1</v>
@@ -45584,10 +45600,10 @@
         <v>0</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>3217</v>
+        <v>3214</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>3218</v>
+        <v>3215</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
@@ -45610,7 +45626,7 @@
         <v>1</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>3209</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -45630,7 +45646,7 @@
         <v>2005</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>3212</v>
+        <v>3209</v>
       </c>
       <c r="H33" s="11" t="b">
         <v>1</v>
@@ -45653,7 +45669,7 @@
         <v>2509</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>3219</v>
+        <v>3216</v>
       </c>
       <c r="H34" s="11" t="b">
         <v>1</v>
@@ -45679,7 +45695,7 @@
         <v>2523</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>3212</v>
+        <v>3209</v>
       </c>
       <c r="H35" s="11" t="b">
         <v>1</v>
@@ -45708,10 +45724,10 @@
         <v>0</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>3220</v>
+        <v>3217</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>3221</v>
+        <v>3218</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -45734,10 +45750,10 @@
         <v>0</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>3222</v>
+        <v>3219</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>3223</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -45763,10 +45779,10 @@
         <v>0</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>3224</v>
+        <v>3221</v>
       </c>
       <c r="J38" s="11" t="s">
-        <v>3225</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -45789,13 +45805,13 @@
         <v>2553</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>3226</v>
+        <v>3223</v>
       </c>
       <c r="H39" s="12" t="b">
         <v>0</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>3218</v>
+        <v>3215</v>
       </c>
     </row>
   </sheetData>
@@ -45815,8 +45831,8 @@
   </sheetPr>
   <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -45833,28 +45849,28 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="22"/>
-      <c r="B1" s="81" t="s">
-        <v>3230</v>
-      </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81" t="s">
-        <v>3231</v>
-      </c>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81" t="s">
-        <v>3232</v>
-      </c>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
+      <c r="B1" s="82" t="s">
+        <v>3227</v>
+      </c>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82" t="s">
+        <v>3228</v>
+      </c>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82" t="s">
+        <v>3229</v>
+      </c>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>3148</v>
+        <v>3147</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>2812</v>
@@ -45863,7 +45879,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>3148</v>
+        <v>3147</v>
       </c>
       <c r="F2" s="22" t="s">
         <v>2812</v>
@@ -45872,7 +45888,7 @@
         <v>3</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>3148</v>
+        <v>3147</v>
       </c>
       <c r="I2" s="22" t="s">
         <v>2812</v>
@@ -45881,13 +45897,13 @@
         <v>3</v>
       </c>
       <c r="K2" s="22" t="s">
+        <v>3131</v>
+      </c>
+      <c r="L2" s="22" t="s">
         <v>3132</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="M2" s="22" t="s">
         <v>3133</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>3134</v>
       </c>
       <c r="N2" s="22" t="s">
         <v>2868</v>
@@ -45928,7 +45944,7 @@
         <v>2814</v>
       </c>
       <c r="K3" s="36" t="s">
-        <v>3135</v>
+        <v>3134</v>
       </c>
       <c r="L3" s="36" t="s">
         <v>2830</v>
@@ -45969,10 +45985,10 @@
         <v>2830</v>
       </c>
       <c r="K4" s="36" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L4" s="42" t="s">
-        <v>3149</v>
+        <v>3148</v>
       </c>
       <c r="M4" s="36">
         <v>1</v>
@@ -46016,10 +46032,10 @@
         <v>2841</v>
       </c>
       <c r="K5" s="36" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>3150</v>
+        <v>3149</v>
       </c>
       <c r="M5" s="36">
         <v>2</v>
@@ -46031,7 +46047,7 @@
         <v>2884</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>3151</v>
+        <v>3150</v>
       </c>
       <c r="Q5" s="11" t="s">
         <v>2885</v>
@@ -46060,10 +46076,10 @@
         <v>2887</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
       <c r="L6" s="42" t="s">
-        <v>3152</v>
+        <v>3151</v>
       </c>
       <c r="M6" s="36">
         <v>4</v>
@@ -46075,7 +46091,7 @@
         <v>2889</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>3153</v>
+        <v>3152</v>
       </c>
       <c r="Q6" s="30" t="s">
         <v>2890</v>
@@ -46104,10 +46120,10 @@
         <v>2887</v>
       </c>
       <c r="K7" s="36" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
       <c r="L7" s="36" t="s">
-        <v>3154</v>
+        <v>3153</v>
       </c>
       <c r="M7" s="36">
         <v>4</v>
@@ -46151,7 +46167,7 @@
         <v>2896</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
       <c r="L8" s="36" t="s">
         <v>2895</v>
@@ -46166,7 +46182,7 @@
         <v>2898</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>3155</v>
+        <v>3154</v>
       </c>
       <c r="Q8" s="11" t="s">
         <v>2899</v>
@@ -46195,7 +46211,7 @@
         <v>2900</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L9" s="36" t="s">
         <v>2804</v>
@@ -46242,7 +46258,7 @@
         <v>2906</v>
       </c>
       <c r="K10" s="36" t="s">
-        <v>3135</v>
+        <v>3134</v>
       </c>
       <c r="L10" s="36" t="s">
         <v>2830</v>
@@ -46257,7 +46273,7 @@
         <v>2908</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>3156</v>
+        <v>3155</v>
       </c>
       <c r="Q10" s="11" t="s">
         <v>2909</v>
@@ -46292,13 +46308,13 @@
         <v>2762</v>
       </c>
       <c r="L11" s="36" t="s">
-        <v>3139</v>
+        <v>3138</v>
       </c>
       <c r="M11" s="36">
         <v>4</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>3157</v>
+        <v>3156</v>
       </c>
       <c r="O11" s="11" t="s">
         <v>2912</v>
@@ -46336,7 +46352,7 @@
         <v>2915</v>
       </c>
       <c r="K12" s="36" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L12" s="36" t="s">
         <v>2830</v>
@@ -46383,7 +46399,7 @@
         <v>2921</v>
       </c>
       <c r="K13" s="36" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L13" s="36" t="s">
         <v>2814</v>
@@ -46427,10 +46443,10 @@
         <v>2926</v>
       </c>
       <c r="K14" s="36" t="s">
+        <v>3136</v>
+      </c>
+      <c r="L14" s="36" t="s">
         <v>3137</v>
-      </c>
-      <c r="L14" s="36" t="s">
-        <v>3138</v>
       </c>
       <c r="M14" s="36">
         <v>4</v>
@@ -46471,10 +46487,10 @@
         <v>2926</v>
       </c>
       <c r="K15" s="36" t="s">
+        <v>3136</v>
+      </c>
+      <c r="L15" s="36" t="s">
         <v>3137</v>
-      </c>
-      <c r="L15" s="36" t="s">
-        <v>3138</v>
       </c>
       <c r="M15" s="36">
         <v>4</v>
@@ -46486,7 +46502,7 @@
         <v>2889</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>3158</v>
+        <v>3157</v>
       </c>
       <c r="Q15" s="11" t="s">
         <v>2890</v>
@@ -46524,7 +46540,7 @@
         <v>2762</v>
       </c>
       <c r="L16" s="36" t="s">
-        <v>3141</v>
+        <v>3140</v>
       </c>
       <c r="M16" s="36">
         <v>4</v>
@@ -46571,10 +46587,10 @@
         <v>2938</v>
       </c>
       <c r="K17" s="36" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L17" s="36" t="s">
-        <v>3142</v>
+        <v>3141</v>
       </c>
       <c r="M17" s="36">
         <v>1</v>
@@ -46612,7 +46628,7 @@
         <v>2841</v>
       </c>
       <c r="K18" s="36" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L18" s="36" t="s">
         <v>2772</v>
@@ -46659,7 +46675,7 @@
         <v>2946</v>
       </c>
       <c r="K19" s="36" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L19" s="36" t="s">
         <v>2825</v>
@@ -46709,7 +46725,7 @@
         <v>2762</v>
       </c>
       <c r="L20" s="36" t="s">
-        <v>3143</v>
+        <v>3142</v>
       </c>
       <c r="M20" s="36">
         <v>2</v>
@@ -46748,7 +46764,7 @@
         <v>2955</v>
       </c>
       <c r="K21" s="36" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L21" s="36" t="s">
         <v>2825</v>
@@ -46797,7 +46813,7 @@
         <v>2960</v>
       </c>
       <c r="K22" s="69" t="s">
-        <v>3144</v>
+        <v>3143</v>
       </c>
       <c r="L22" s="69" t="s">
         <v>2824</v>
@@ -46848,7 +46864,7 @@
         <v>2964</v>
       </c>
       <c r="K23" s="69" t="s">
-        <v>3135</v>
+        <v>3134</v>
       </c>
       <c r="L23" s="69" t="s">
         <v>2824</v>
@@ -46861,7 +46877,7 @@
         <v>2966</v>
       </c>
       <c r="P23" s="70" t="s">
-        <v>3159</v>
+        <v>3158</v>
       </c>
       <c r="Q23" s="64" t="s">
         <v>2904</v>
@@ -46901,7 +46917,7 @@
         <v>2967</v>
       </c>
       <c r="K24" s="38" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L24" s="38" t="s">
         <v>2830</v>
@@ -46909,8 +46925,8 @@
       <c r="M24" s="38">
         <v>3</v>
       </c>
-      <c r="N24" s="44" t="s">
-        <v>2904</v>
+      <c r="N24" s="32" t="s">
+        <v>3238</v>
       </c>
       <c r="O24" s="44" t="s">
         <v>2962</v>
@@ -46951,13 +46967,13 @@
       </c>
       <c r="I25" s="47"/>
       <c r="J25" s="47" t="s">
-        <v>3160</v>
+        <v>3159</v>
       </c>
       <c r="K25" s="49" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L25" s="49" t="s">
-        <v>2824</v>
+        <v>3231</v>
       </c>
       <c r="M25" s="50"/>
       <c r="N25" s="51" t="s">
@@ -47000,7 +47016,7 @@
       </c>
       <c r="I26" s="11"/>
       <c r="K26" s="36" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L26" s="36" t="s">
         <v>2819</v>
@@ -47042,7 +47058,7 @@
       </c>
       <c r="I27" s="11"/>
       <c r="K27" s="36" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L27" s="36" t="s">
         <v>2819</v>
@@ -47089,7 +47105,7 @@
         <v>2976</v>
       </c>
       <c r="K28" s="36" t="s">
-        <v>3135</v>
+        <v>3134</v>
       </c>
       <c r="L28" s="36" t="s">
         <v>2814</v>
@@ -47134,7 +47150,7 @@
       </c>
       <c r="I29" s="11"/>
       <c r="K29" s="36" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
       <c r="L29" s="36" t="s">
         <v>2819</v>
@@ -47149,7 +47165,7 @@
         <v>2980</v>
       </c>
       <c r="P29" s="21" t="s">
-        <v>3161</v>
+        <v>3160</v>
       </c>
       <c r="Q29" s="11" t="s">
         <v>2904</v>
@@ -47179,10 +47195,10 @@
       <c r="I30" s="47"/>
       <c r="J30" s="48"/>
       <c r="K30" s="49" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
       <c r="L30" s="49" t="s">
-        <v>3162</v>
+        <v>3232</v>
       </c>
       <c r="M30" s="49"/>
       <c r="N30" s="52" t="s">
@@ -47225,7 +47241,7 @@
         <v>2982</v>
       </c>
       <c r="K31" s="36" t="s">
-        <v>3144</v>
+        <v>3143</v>
       </c>
       <c r="L31" s="36" t="s">
         <v>2819</v>
@@ -47240,7 +47256,7 @@
         <v>2889</v>
       </c>
       <c r="P31" s="21" t="s">
-        <v>3163</v>
+        <v>3161</v>
       </c>
       <c r="Q31" s="11" t="s">
         <v>2904</v>
@@ -47285,7 +47301,7 @@
         <v>2985</v>
       </c>
       <c r="P32" s="21" t="s">
-        <v>3164</v>
+        <v>3162</v>
       </c>
       <c r="Q32" s="11" t="s">
         <v>2904</v>
@@ -47330,7 +47346,7 @@
         <v>2988</v>
       </c>
       <c r="P33" s="70" t="s">
-        <v>3165</v>
+        <v>3163</v>
       </c>
       <c r="Q33" s="64" t="s">
         <v>2904</v>
@@ -47381,7 +47397,7 @@
         <v>2985</v>
       </c>
       <c r="P34" s="21" t="s">
-        <v>3166</v>
+        <v>3164</v>
       </c>
       <c r="Q34" s="11" t="s">
         <v>2904</v>
@@ -47413,7 +47429,7 @@
         <v>2990</v>
       </c>
       <c r="K35" s="37" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L35" s="37" t="s">
         <v>2819</v>
@@ -47482,7 +47498,7 @@
         <v>2917</v>
       </c>
       <c r="P36" s="21" t="s">
-        <v>3167</v>
+        <v>3165</v>
       </c>
       <c r="Q36" s="11" t="s">
         <v>2904</v>
@@ -47511,10 +47527,12 @@
       </c>
       <c r="I37" s="47"/>
       <c r="J37" s="47" t="s">
-        <v>3168</v>
+        <v>3166</v>
       </c>
       <c r="K37" s="50"/>
-      <c r="L37" s="50"/>
+      <c r="L37" s="50" t="s">
+        <v>3233</v>
+      </c>
       <c r="M37" s="50"/>
       <c r="N37" s="52" t="s">
         <v>2996</v>
@@ -47572,8 +47590,8 @@
       <c r="M38" s="36">
         <v>4</v>
       </c>
-      <c r="N38" s="11" t="s">
-        <v>2904</v>
+      <c r="N38" s="32" t="s">
+        <v>3238</v>
       </c>
       <c r="O38" s="11" t="s">
         <v>2999</v>
@@ -47613,7 +47631,7 @@
         <v>3002</v>
       </c>
       <c r="K39" s="69" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
       <c r="L39" s="69" t="s">
         <v>2814</v>
@@ -47664,7 +47682,9 @@
         <v>3006</v>
       </c>
       <c r="K40" s="49"/>
-      <c r="L40" s="49"/>
+      <c r="L40" s="49" t="s">
+        <v>3235</v>
+      </c>
       <c r="M40" s="49"/>
       <c r="N40" s="52" t="s">
         <v>3007</v>
@@ -47711,7 +47731,7 @@
       </c>
       <c r="J41" s="7"/>
       <c r="K41" s="36" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L41" s="36" t="s">
         <v>2838</v>
@@ -47755,7 +47775,7 @@
         <v>3014</v>
       </c>
       <c r="K42" s="36" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
       <c r="L42" s="36" t="s">
         <v>2814</v>
@@ -47800,7 +47820,7 @@
       <c r="I43" s="64"/>
       <c r="J43" s="62"/>
       <c r="K43" s="69" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L43" s="69" t="s">
         <v>2824</v>
@@ -47902,7 +47922,7 @@
         <v>2970</v>
       </c>
       <c r="P45" s="21" t="s">
-        <v>3169</v>
+        <v>3167</v>
       </c>
       <c r="Q45" s="11" t="s">
         <v>2904</v>
@@ -47932,10 +47952,10 @@
       <c r="I46" s="47"/>
       <c r="J46" s="48"/>
       <c r="K46" s="49" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L46" s="49" t="s">
-        <v>3170</v>
+        <v>3234</v>
       </c>
       <c r="M46" s="53"/>
       <c r="N46" s="52" t="s">
@@ -47945,7 +47965,7 @@
         <v>3027</v>
       </c>
       <c r="P46" s="54" t="s">
-        <v>3171</v>
+        <v>3168</v>
       </c>
       <c r="Q46" s="47" t="s">
         <v>2904</v>
@@ -47995,7 +48015,7 @@
         <v>3031</v>
       </c>
       <c r="P47" s="21" t="s">
-        <v>3172</v>
+        <v>3169</v>
       </c>
       <c r="Q47" s="11" t="s">
         <v>2904</v>
@@ -48024,7 +48044,7 @@
         <v>2809</v>
       </c>
       <c r="K48" s="36" t="s">
-        <v>3135</v>
+        <v>3134</v>
       </c>
       <c r="L48" s="36" t="s">
         <v>2809</v>
@@ -48039,7 +48059,7 @@
         <v>2970</v>
       </c>
       <c r="P48" s="21" t="s">
-        <v>3173</v>
+        <v>3170</v>
       </c>
       <c r="Q48" s="11" t="s">
         <v>2904</v>
@@ -48068,7 +48088,7 @@
         <v>3033</v>
       </c>
       <c r="K49" s="36" t="s">
-        <v>3145</v>
+        <v>3144</v>
       </c>
       <c r="L49" s="36" t="s">
         <v>2830</v>
@@ -48109,7 +48129,7 @@
         <v>2814</v>
       </c>
       <c r="K50" s="36" t="s">
-        <v>3135</v>
+        <v>3134</v>
       </c>
       <c r="L50" s="36" t="s">
         <v>2814</v>
@@ -48156,7 +48176,9 @@
       </c>
       <c r="J51" s="75"/>
       <c r="K51" s="77"/>
-      <c r="L51" s="77"/>
+      <c r="L51" s="53" t="s">
+        <v>3236</v>
+      </c>
       <c r="M51" s="78"/>
       <c r="N51" s="75"/>
       <c r="O51" s="75"/>
@@ -48194,7 +48216,7 @@
         <v>3042</v>
       </c>
       <c r="K52" s="36" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L52" s="36" t="s">
         <v>2809</v>
@@ -48250,7 +48272,7 @@
         <v>2944</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>3174</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
@@ -48276,7 +48298,7 @@
         <v>3042</v>
       </c>
       <c r="K54" s="36" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L54" s="36" t="s">
         <v>2809</v>
@@ -48367,7 +48389,7 @@
         <v>3052</v>
       </c>
       <c r="K56" s="36" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
       <c r="L56" s="36" t="s">
         <v>2819</v>
@@ -48382,7 +48404,7 @@
         <v>2923</v>
       </c>
       <c r="P56" s="21" t="s">
-        <v>3175</v>
+        <v>3172</v>
       </c>
       <c r="Q56" s="11" t="s">
         <v>2904</v>
@@ -48408,7 +48430,7 @@
         <v>2830</v>
       </c>
       <c r="K57" s="36" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L57" s="36" t="s">
         <v>2830</v>
@@ -48452,7 +48474,7 @@
         <v>3056</v>
       </c>
       <c r="K58" s="36" t="s">
-        <v>3144</v>
+        <v>3143</v>
       </c>
       <c r="L58" s="36" t="s">
         <v>2819</v>
@@ -48499,7 +48521,7 @@
         <v>2762</v>
       </c>
       <c r="L59" s="36" t="s">
-        <v>3146</v>
+        <v>3145</v>
       </c>
       <c r="M59" s="36">
         <v>3</v>
@@ -48511,7 +48533,7 @@
         <v>3060</v>
       </c>
       <c r="P59" s="21" t="s">
-        <v>3176</v>
+        <v>3173</v>
       </c>
       <c r="Q59" s="11" t="s">
         <v>2904</v>
@@ -48543,7 +48565,7 @@
         <v>3062</v>
       </c>
       <c r="K60" s="36" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L60" s="36" t="s">
         <v>2814</v>
@@ -48587,7 +48609,7 @@
         <v>3067</v>
       </c>
       <c r="K61" s="36" t="s">
-        <v>3144</v>
+        <v>3143</v>
       </c>
       <c r="L61" s="36" t="s">
         <v>2819</v>
@@ -48628,7 +48650,7 @@
         <v>2755</v>
       </c>
       <c r="K62" s="36" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L62" s="36" t="s">
         <v>2830</v>
@@ -48643,7 +48665,7 @@
         <v>3072</v>
       </c>
       <c r="P62" s="21" t="s">
-        <v>3177</v>
+        <v>3174</v>
       </c>
       <c r="Q62" s="11" t="s">
         <v>2881</v>
@@ -48673,14 +48695,14 @@
       <c r="I63" s="64"/>
       <c r="J63" s="62"/>
       <c r="K63" s="69" t="s">
-        <v>3145</v>
+        <v>3144</v>
       </c>
       <c r="L63" s="69" t="s">
         <v>2824</v>
       </c>
       <c r="M63" s="69"/>
       <c r="N63" s="70" t="s">
-        <v>3178</v>
+        <v>3175</v>
       </c>
       <c r="O63" s="64" t="s">
         <v>3073</v>
@@ -48725,7 +48747,7 @@
         <v>3076</v>
       </c>
       <c r="K64" s="36" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L64" s="36" t="s">
         <v>2777</v>
@@ -48769,7 +48791,7 @@
         <v>3066</v>
       </c>
       <c r="K65" s="36" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L65" s="36" t="s">
         <v>2819</v>
@@ -48784,7 +48806,7 @@
         <v>2902</v>
       </c>
       <c r="P65" s="21" t="s">
-        <v>3179</v>
+        <v>3176</v>
       </c>
       <c r="Q65" s="11" t="s">
         <v>2904</v>
@@ -48873,7 +48895,7 @@
         <v>3080</v>
       </c>
       <c r="K67" s="37" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L67" s="37" t="s">
         <v>2819</v>
@@ -48926,7 +48948,7 @@
         <v>3085</v>
       </c>
       <c r="K68" s="36" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L68" s="36" t="s">
         <v>2814</v>
@@ -48973,7 +48995,7 @@
         <v>3066</v>
       </c>
       <c r="K69" s="36" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L69" s="36" t="s">
         <v>2819</v>
@@ -48988,7 +49010,7 @@
         <v>2879</v>
       </c>
       <c r="P69" s="21" t="s">
-        <v>3180</v>
+        <v>3177</v>
       </c>
       <c r="Q69" s="11" t="s">
         <v>2904</v>
@@ -49076,7 +49098,7 @@
         <v>2762</v>
       </c>
       <c r="L71" s="42" t="s">
-        <v>3181</v>
+        <v>3178</v>
       </c>
       <c r="M71" s="36">
         <v>4</v>
@@ -49115,7 +49137,7 @@
       </c>
       <c r="I72" s="11"/>
       <c r="K72" s="36" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
       <c r="L72" s="36" t="s">
         <v>2819</v>
@@ -49130,7 +49152,7 @@
         <v>2889</v>
       </c>
       <c r="P72" s="21" t="s">
-        <v>3182</v>
+        <v>3179</v>
       </c>
       <c r="Q72" s="11" t="s">
         <v>2904</v>
@@ -49160,7 +49182,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="7"/>
       <c r="K73" s="37" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L73" s="37" t="s">
         <v>2814</v>
@@ -49217,7 +49239,7 @@
         <v>3080</v>
       </c>
       <c r="K74" s="37" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L74" s="37" t="s">
         <v>2841</v>
@@ -49317,7 +49339,7 @@
       </c>
       <c r="I76" s="11"/>
       <c r="K76" s="36" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L76" s="36" t="s">
         <v>2804</v>
@@ -49364,7 +49386,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="7"/>
       <c r="K77" s="37" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="L77" s="37" t="s">
         <v>2804</v>
@@ -49429,7 +49451,7 @@
         <v>3</v>
       </c>
       <c r="N78" s="11" t="s">
-        <v>2904</v>
+        <v>3237</v>
       </c>
       <c r="O78" s="11">
         <v>2.2000000000000002</v>
@@ -49467,7 +49489,7 @@
         <v>3113</v>
       </c>
       <c r="K79" s="37" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L79" s="37" t="s">
         <v>2838</v>
@@ -49475,14 +49497,14 @@
       <c r="M79" s="37">
         <v>2</v>
       </c>
-      <c r="N79" s="8" t="s">
-        <v>3114</v>
+      <c r="N79" s="26" t="s">
+        <v>2410</v>
       </c>
       <c r="O79" s="8" t="s">
         <v>3073</v>
       </c>
       <c r="P79" s="8" t="s">
-        <v>3115</v>
+        <v>3114</v>
       </c>
       <c r="Q79" s="8" t="s">
         <v>2904</v>
@@ -49511,29 +49533,29 @@
         <v>2866</v>
       </c>
       <c r="H80" s="40" t="s">
-        <v>3116</v>
+        <v>3115</v>
       </c>
       <c r="I80" s="11"/>
       <c r="J80" s="11" t="s">
-        <v>3117</v>
+        <v>3116</v>
       </c>
       <c r="K80" s="36" t="s">
         <v>2762</v>
       </c>
       <c r="L80" s="36" t="s">
-        <v>3147</v>
+        <v>3146</v>
       </c>
       <c r="M80" s="36">
         <v>4</v>
       </c>
       <c r="N80" s="10" t="s">
+        <v>3117</v>
+      </c>
+      <c r="O80" s="11" t="s">
         <v>3118</v>
       </c>
-      <c r="O80" s="11" t="s">
-        <v>3119</v>
-      </c>
       <c r="P80" s="21" t="s">
-        <v>3183</v>
+        <v>3180</v>
       </c>
       <c r="Q80" s="11" t="s">
         <v>2904</v>
@@ -49562,7 +49584,7 @@
         <v>3014</v>
       </c>
       <c r="K81" s="36" t="s">
-        <v>3145</v>
+        <v>3144</v>
       </c>
       <c r="L81" s="36" t="s">
         <v>2814</v>
@@ -49571,13 +49593,13 @@
         <v>2</v>
       </c>
       <c r="N81" s="11" t="s">
+        <v>3119</v>
+      </c>
+      <c r="O81" s="11" t="s">
         <v>3120</v>
       </c>
-      <c r="O81" s="11" t="s">
+      <c r="P81" s="11" t="s">
         <v>3121</v>
-      </c>
-      <c r="P81" s="11" t="s">
-        <v>3122</v>
       </c>
       <c r="Q81" s="11" t="s">
         <v>2904</v>
@@ -49603,10 +49625,10 @@
         <v>2993</v>
       </c>
       <c r="I82" s="11" t="s">
+        <v>3122</v>
+      </c>
+      <c r="J82" s="11" t="s">
         <v>3123</v>
-      </c>
-      <c r="J82" s="11" t="s">
-        <v>3124</v>
       </c>
       <c r="K82" s="36" t="s">
         <v>2762</v>
@@ -49618,7 +49640,7 @@
         <v>4</v>
       </c>
       <c r="N82" s="11" t="s">
-        <v>3125</v>
+        <v>3124</v>
       </c>
       <c r="O82" s="11" t="s">
         <v>2944</v>
@@ -49627,7 +49649,7 @@
         <v>3083</v>
       </c>
       <c r="Q82" s="11" t="s">
-        <v>3126</v>
+        <v>3125</v>
       </c>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.2">
@@ -49656,7 +49678,7 @@
       </c>
       <c r="J83" s="7"/>
       <c r="K83" s="37" t="s">
-        <v>3140</v>
+        <v>3139</v>
       </c>
       <c r="L83" s="37" t="s">
         <v>2826</v>
@@ -49671,7 +49693,7 @@
         <v>2962</v>
       </c>
       <c r="P83" s="55" t="s">
-        <v>3184</v>
+        <v>3181</v>
       </c>
       <c r="Q83" s="8" t="s">
         <v>2904</v>
@@ -49715,16 +49737,16 @@
         <v>4</v>
       </c>
       <c r="N84" s="10" t="s">
+        <v>3126</v>
+      </c>
+      <c r="O84" s="11" t="s">
         <v>3127</v>
-      </c>
-      <c r="O84" s="11" t="s">
-        <v>3128</v>
       </c>
       <c r="P84" s="11" t="s">
         <v>2970</v>
       </c>
       <c r="Q84" s="11" t="s">
-        <v>3129</v>
+        <v>3128</v>
       </c>
     </row>
     <row r="85" spans="1:23" s="66" customFormat="1" x14ac:dyDescent="0.2">
@@ -49749,7 +49771,7 @@
         <v>2820</v>
       </c>
       <c r="I85" s="64" t="s">
-        <v>3130</v>
+        <v>3129</v>
       </c>
       <c r="J85" s="62"/>
       <c r="K85" s="69" t="s">
@@ -49763,7 +49785,7 @@
         <v>2519</v>
       </c>
       <c r="O85" s="64" t="s">
-        <v>3131</v>
+        <v>3130</v>
       </c>
       <c r="P85" s="64">
         <v>1.1399999999999999</v>
@@ -49785,7 +49807,7 @@
     </row>
     <row r="87" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A87" s="80" t="s">
-        <v>3233</v>
+        <v>3230</v>
       </c>
       <c r="B87" s="56"/>
       <c r="E87" s="56"/>

</xml_diff>